<commit_message>
Store page aur scraping logic ko restore kiya, extra code remove kiya
</commit_message>
<xml_diff>
--- a/user_export.xlsx
+++ b/user_export.xlsx
@@ -490,12 +490,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ABDUL SATTAR</t>
+          <t>abdul  ghaffar</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>BR</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -508,7 +508,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Diamond</t>
+          <t>Immortal</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">

</xml_diff>